<commit_message>
updates to pintle design documents
</commit_message>
<xml_diff>
--- a/Pintle/Pintle Injector Design Documentation/Pintle_V3_python_hand_calcs.xlsx
+++ b/Pintle/Pintle Injector Design Documentation/Pintle_V3_python_hand_calcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jntil\Documents\Git_Repos\liquid-engine-test-stand\Pintle\Pintle Injector Design Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9286DFA-4810-448D-B618-7738361620E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D69A4B-5DE2-4984-8543-F8B4B7CE6D08}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15525" yWindow="1290" windowWidth="6630" windowHeight="7770" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" firstSheet="7" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Injector V3 mjp T4A" sheetId="8" r:id="rId1"/>
@@ -1368,20 +1368,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="44" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1407,6 +1401,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="48" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="44" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1819,20 +1819,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="101"/>
+      <c r="B1" s="114"/>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="100" t="s">
+      <c r="F1" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="101"/>
+      <c r="G1" s="114"/>
       <c r="H1" s="8" t="s">
         <v>1</v>
       </c>
@@ -1929,10 +1929,10 @@
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="105"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="6">
         <v>12</v>
       </c>
@@ -1951,10 +1951,10 @@
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="105"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="7">
         <v>0.57613333318776305</v>
       </c>
@@ -2016,41 +2016,41 @@
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="106" t="s">
+      <c r="A11" s="104" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="106"/>
-      <c r="C11" s="106"/>
-      <c r="D11" s="106"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="106"/>
-      <c r="G11" s="106"/>
-      <c r="H11" s="106"/>
-      <c r="I11" s="106"/>
-      <c r="J11" s="106"/>
-      <c r="K11" s="106"/>
-      <c r="L11" s="106"/>
-      <c r="M11" s="108" t="s">
+      <c r="B11" s="104"/>
+      <c r="C11" s="104"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="104"/>
+      <c r="F11" s="104"/>
+      <c r="G11" s="104"/>
+      <c r="H11" s="104"/>
+      <c r="I11" s="104"/>
+      <c r="J11" s="104"/>
+      <c r="K11" s="104"/>
+      <c r="L11" s="104"/>
+      <c r="M11" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="N11" s="109"/>
-      <c r="O11" s="109"/>
-      <c r="P11" s="109"/>
-      <c r="Q11" s="109"/>
-      <c r="R11" s="109"/>
-      <c r="S11" s="109"/>
-      <c r="T11" s="109"/>
-      <c r="U11" s="109"/>
-      <c r="V11" s="110"/>
-      <c r="W11" s="114" t="s">
+      <c r="N11" s="107"/>
+      <c r="O11" s="107"/>
+      <c r="P11" s="107"/>
+      <c r="Q11" s="107"/>
+      <c r="R11" s="107"/>
+      <c r="S11" s="107"/>
+      <c r="T11" s="107"/>
+      <c r="U11" s="107"/>
+      <c r="V11" s="108"/>
+      <c r="W11" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="X11" s="114"/>
-      <c r="Y11" s="114"/>
-      <c r="Z11" s="114"/>
-      <c r="AA11" s="114"/>
-      <c r="AB11" s="114"/>
-      <c r="AC11" s="114"/>
+      <c r="X11" s="112"/>
+      <c r="Y11" s="112"/>
+      <c r="Z11" s="112"/>
+      <c r="AA11" s="112"/>
+      <c r="AB11" s="112"/>
+      <c r="AC11" s="112"/>
     </row>
     <row r="12" spans="1:29" s="1" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
@@ -2651,43 +2651,43 @@
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A24" s="107" t="s">
+      <c r="A24" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="107"/>
-      <c r="C24" s="107"/>
-      <c r="D24" s="107"/>
-      <c r="E24" s="107"/>
-      <c r="F24" s="107"/>
-      <c r="G24" s="107"/>
-      <c r="H24" s="107"/>
-      <c r="I24" s="107"/>
-      <c r="J24" s="107"/>
-      <c r="K24" s="107"/>
-      <c r="L24" s="107"/>
-      <c r="M24" s="111" t="s">
+      <c r="B24" s="105"/>
+      <c r="C24" s="105"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="105"/>
+      <c r="F24" s="105"/>
+      <c r="G24" s="105"/>
+      <c r="H24" s="105"/>
+      <c r="I24" s="105"/>
+      <c r="J24" s="105"/>
+      <c r="K24" s="105"/>
+      <c r="L24" s="105"/>
+      <c r="M24" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="N24" s="112"/>
-      <c r="O24" s="112"/>
-      <c r="P24" s="112"/>
-      <c r="Q24" s="112"/>
-      <c r="R24" s="112"/>
-      <c r="S24" s="112"/>
-      <c r="T24" s="112"/>
-      <c r="U24" s="112"/>
-      <c r="V24" s="112"/>
-      <c r="W24" s="112"/>
-      <c r="X24" s="113"/>
-      <c r="Y24" s="114" t="s">
+      <c r="N24" s="110"/>
+      <c r="O24" s="110"/>
+      <c r="P24" s="110"/>
+      <c r="Q24" s="110"/>
+      <c r="R24" s="110"/>
+      <c r="S24" s="110"/>
+      <c r="T24" s="110"/>
+      <c r="U24" s="110"/>
+      <c r="V24" s="110"/>
+      <c r="W24" s="110"/>
+      <c r="X24" s="111"/>
+      <c r="Y24" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="Z24" s="114"/>
-      <c r="AA24" s="114"/>
-      <c r="AB24" s="114"/>
-      <c r="AC24" s="114"/>
-      <c r="AD24" s="114"/>
-      <c r="AE24" s="114"/>
+      <c r="Z24" s="112"/>
+      <c r="AA24" s="112"/>
+      <c r="AB24" s="112"/>
+      <c r="AC24" s="112"/>
+      <c r="AD24" s="112"/>
+      <c r="AE24" s="112"/>
     </row>
     <row r="25" spans="1:31" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
@@ -3362,6 +3362,18 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="A11:L11"/>
@@ -3370,18 +3382,6 @@
     <mergeCell ref="M24:X24"/>
     <mergeCell ref="W11:AC11"/>
     <mergeCell ref="Y24:AE24"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3417,20 +3417,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="101"/>
+      <c r="B1" s="114"/>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="100" t="s">
+      <c r="F1" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="101"/>
+      <c r="G1" s="114"/>
       <c r="H1" s="8" t="s">
         <v>1</v>
       </c>
@@ -3527,10 +3527,10 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="105"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="6">
         <v>12</v>
       </c>
@@ -3549,10 +3549,10 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="105"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="6">
         <v>0.54</v>
       </c>
@@ -3628,18 +3628,18 @@
       <c r="J11" s="125"/>
       <c r="K11" s="125"/>
       <c r="L11" s="125"/>
-      <c r="M11" s="108" t="s">
+      <c r="M11" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="N11" s="109"/>
-      <c r="O11" s="109"/>
-      <c r="P11" s="109"/>
-      <c r="Q11" s="109"/>
-      <c r="R11" s="109"/>
-      <c r="S11" s="109"/>
-      <c r="T11" s="109"/>
-      <c r="U11" s="109"/>
-      <c r="V11" s="110"/>
+      <c r="N11" s="107"/>
+      <c r="O11" s="107"/>
+      <c r="P11" s="107"/>
+      <c r="Q11" s="107"/>
+      <c r="R11" s="107"/>
+      <c r="S11" s="107"/>
+      <c r="T11" s="107"/>
+      <c r="U11" s="107"/>
+      <c r="V11" s="108"/>
     </row>
     <row r="12" spans="1:22" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -6649,6 +6649,16 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="M11:V11"/>
+    <mergeCell ref="A47:L47"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:L11"/>
+    <mergeCell ref="M47:X47"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="A7:B7"/>
@@ -6657,16 +6667,6 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="M11:V11"/>
-    <mergeCell ref="A47:L47"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="M47:X47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6694,10 +6694,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="101"/>
+      <c r="B1" s="114"/>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
@@ -6754,10 +6754,10 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="105"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="6">
         <v>12</v>
       </c>
@@ -6766,10 +6766,10 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="105"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="6">
         <v>0.54</v>
       </c>
@@ -9017,12 +9017,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A42:B42"/>
@@ -9030,6 +9024,12 @@
     <mergeCell ref="A44:B44"/>
     <mergeCell ref="A45:B45"/>
     <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9695,8 +9695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7151EEB2-A148-497B-8F06-60E1B180A556}">
   <dimension ref="A2:AP103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F89" sqref="F88:F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10336,7 +10336,7 @@
         <v>1.5</v>
       </c>
       <c r="AK12" s="99">
-        <f t="shared" ref="AK10:AK12" si="4">AD12+0.02</f>
+        <f t="shared" ref="AK12" si="4">AD12+0.02</f>
         <v>0.14000000000000001</v>
       </c>
       <c r="AL12" s="99">
@@ -10381,7 +10381,7 @@
         <v>4</v>
       </c>
       <c r="I13" s="88">
-        <f t="shared" ref="I13:N13" si="5">B10</f>
+        <f t="shared" ref="I13:M13" si="5">B10</f>
         <v>0.06</v>
       </c>
       <c r="J13" s="88">
@@ -13702,20 +13702,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="101"/>
+      <c r="B1" s="114"/>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="100" t="s">
+      <c r="F1" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="101"/>
+      <c r="G1" s="114"/>
       <c r="H1" s="8" t="s">
         <v>1</v>
       </c>
@@ -13812,10 +13812,10 @@
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="105"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="6">
         <v>12</v>
       </c>
@@ -13834,10 +13834,10 @@
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="105"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="7">
         <v>0.53984146967987301</v>
       </c>
@@ -13900,41 +13900,41 @@
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="106" t="s">
+      <c r="A11" s="104" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="106"/>
-      <c r="C11" s="106"/>
-      <c r="D11" s="106"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="106"/>
-      <c r="G11" s="106"/>
-      <c r="H11" s="106"/>
-      <c r="I11" s="106"/>
-      <c r="J11" s="106"/>
-      <c r="K11" s="106"/>
-      <c r="L11" s="106"/>
-      <c r="M11" s="108" t="s">
+      <c r="B11" s="104"/>
+      <c r="C11" s="104"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="104"/>
+      <c r="F11" s="104"/>
+      <c r="G11" s="104"/>
+      <c r="H11" s="104"/>
+      <c r="I11" s="104"/>
+      <c r="J11" s="104"/>
+      <c r="K11" s="104"/>
+      <c r="L11" s="104"/>
+      <c r="M11" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="N11" s="109"/>
-      <c r="O11" s="109"/>
-      <c r="P11" s="109"/>
-      <c r="Q11" s="109"/>
-      <c r="R11" s="109"/>
-      <c r="S11" s="109"/>
-      <c r="T11" s="109"/>
-      <c r="U11" s="109"/>
-      <c r="V11" s="110"/>
-      <c r="W11" s="114" t="s">
+      <c r="N11" s="107"/>
+      <c r="O11" s="107"/>
+      <c r="P11" s="107"/>
+      <c r="Q11" s="107"/>
+      <c r="R11" s="107"/>
+      <c r="S11" s="107"/>
+      <c r="T11" s="107"/>
+      <c r="U11" s="107"/>
+      <c r="V11" s="108"/>
+      <c r="W11" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="X11" s="114"/>
-      <c r="Y11" s="114"/>
-      <c r="Z11" s="114"/>
-      <c r="AA11" s="114"/>
-      <c r="AB11" s="114"/>
-      <c r="AC11" s="114"/>
+      <c r="X11" s="112"/>
+      <c r="Y11" s="112"/>
+      <c r="Z11" s="112"/>
+      <c r="AA11" s="112"/>
+      <c r="AB11" s="112"/>
+      <c r="AC11" s="112"/>
     </row>
     <row r="12" spans="1:29" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
@@ -14933,43 +14933,43 @@
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A29" s="107" t="s">
+      <c r="A29" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="107"/>
-      <c r="C29" s="107"/>
-      <c r="D29" s="107"/>
-      <c r="E29" s="107"/>
-      <c r="F29" s="107"/>
-      <c r="G29" s="107"/>
-      <c r="H29" s="107"/>
-      <c r="I29" s="107"/>
-      <c r="J29" s="107"/>
-      <c r="K29" s="107"/>
-      <c r="L29" s="107"/>
-      <c r="M29" s="111" t="s">
+      <c r="B29" s="105"/>
+      <c r="C29" s="105"/>
+      <c r="D29" s="105"/>
+      <c r="E29" s="105"/>
+      <c r="F29" s="105"/>
+      <c r="G29" s="105"/>
+      <c r="H29" s="105"/>
+      <c r="I29" s="105"/>
+      <c r="J29" s="105"/>
+      <c r="K29" s="105"/>
+      <c r="L29" s="105"/>
+      <c r="M29" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="N29" s="112"/>
-      <c r="O29" s="112"/>
-      <c r="P29" s="112"/>
-      <c r="Q29" s="112"/>
-      <c r="R29" s="112"/>
-      <c r="S29" s="112"/>
-      <c r="T29" s="112"/>
-      <c r="U29" s="112"/>
-      <c r="V29" s="112"/>
-      <c r="W29" s="112"/>
-      <c r="X29" s="113"/>
-      <c r="Y29" s="114" t="s">
+      <c r="N29" s="110"/>
+      <c r="O29" s="110"/>
+      <c r="P29" s="110"/>
+      <c r="Q29" s="110"/>
+      <c r="R29" s="110"/>
+      <c r="S29" s="110"/>
+      <c r="T29" s="110"/>
+      <c r="U29" s="110"/>
+      <c r="V29" s="110"/>
+      <c r="W29" s="110"/>
+      <c r="X29" s="111"/>
+      <c r="Y29" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="Z29" s="114"/>
-      <c r="AA29" s="114"/>
-      <c r="AB29" s="114"/>
-      <c r="AC29" s="114"/>
-      <c r="AD29" s="114"/>
-      <c r="AE29" s="114"/>
+      <c r="Z29" s="112"/>
+      <c r="AA29" s="112"/>
+      <c r="AB29" s="112"/>
+      <c r="AC29" s="112"/>
+      <c r="AD29" s="112"/>
+      <c r="AE29" s="112"/>
     </row>
     <row r="30" spans="1:31" s="1" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
@@ -16016,6 +16016,18 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="A11:L11"/>
     <mergeCell ref="A29:L29"/>
     <mergeCell ref="M29:X29"/>
@@ -16024,18 +16036,6 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="W11:AC11"/>
     <mergeCell ref="Y29:AE29"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16067,20 +16067,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="101"/>
+      <c r="B1" s="114"/>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="100" t="s">
+      <c r="F1" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="101"/>
+      <c r="G1" s="114"/>
       <c r="H1" s="8" t="s">
         <v>1</v>
       </c>
@@ -16177,10 +16177,10 @@
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="105"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="6">
         <v>12</v>
       </c>
@@ -16199,10 +16199,10 @@
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="105"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="7">
         <v>0.55345091849533101</v>
       </c>
@@ -16265,41 +16265,41 @@
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="106" t="s">
+      <c r="A11" s="104" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="106"/>
-      <c r="C11" s="106"/>
-      <c r="D11" s="106"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="106"/>
-      <c r="G11" s="106"/>
-      <c r="H11" s="106"/>
-      <c r="I11" s="106"/>
-      <c r="J11" s="106"/>
-      <c r="K11" s="106"/>
-      <c r="L11" s="106"/>
-      <c r="M11" s="108" t="s">
+      <c r="B11" s="104"/>
+      <c r="C11" s="104"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="104"/>
+      <c r="F11" s="104"/>
+      <c r="G11" s="104"/>
+      <c r="H11" s="104"/>
+      <c r="I11" s="104"/>
+      <c r="J11" s="104"/>
+      <c r="K11" s="104"/>
+      <c r="L11" s="104"/>
+      <c r="M11" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="N11" s="109"/>
-      <c r="O11" s="109"/>
-      <c r="P11" s="109"/>
-      <c r="Q11" s="109"/>
-      <c r="R11" s="109"/>
-      <c r="S11" s="109"/>
-      <c r="T11" s="109"/>
-      <c r="U11" s="109"/>
-      <c r="V11" s="110"/>
-      <c r="W11" s="114" t="s">
+      <c r="N11" s="107"/>
+      <c r="O11" s="107"/>
+      <c r="P11" s="107"/>
+      <c r="Q11" s="107"/>
+      <c r="R11" s="107"/>
+      <c r="S11" s="107"/>
+      <c r="T11" s="107"/>
+      <c r="U11" s="107"/>
+      <c r="V11" s="108"/>
+      <c r="W11" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="X11" s="114"/>
-      <c r="Y11" s="114"/>
-      <c r="Z11" s="114"/>
-      <c r="AA11" s="114"/>
-      <c r="AB11" s="114"/>
-      <c r="AC11" s="114"/>
+      <c r="X11" s="112"/>
+      <c r="Y11" s="112"/>
+      <c r="Z11" s="112"/>
+      <c r="AA11" s="112"/>
+      <c r="AB11" s="112"/>
+      <c r="AC11" s="112"/>
     </row>
     <row r="12" spans="1:29" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
@@ -17250,43 +17250,43 @@
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A29" s="107" t="s">
+      <c r="A29" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="107"/>
-      <c r="C29" s="107"/>
-      <c r="D29" s="107"/>
-      <c r="E29" s="107"/>
-      <c r="F29" s="107"/>
-      <c r="G29" s="107"/>
-      <c r="H29" s="107"/>
-      <c r="I29" s="107"/>
-      <c r="J29" s="107"/>
-      <c r="K29" s="107"/>
-      <c r="L29" s="107"/>
-      <c r="M29" s="111" t="s">
+      <c r="B29" s="105"/>
+      <c r="C29" s="105"/>
+      <c r="D29" s="105"/>
+      <c r="E29" s="105"/>
+      <c r="F29" s="105"/>
+      <c r="G29" s="105"/>
+      <c r="H29" s="105"/>
+      <c r="I29" s="105"/>
+      <c r="J29" s="105"/>
+      <c r="K29" s="105"/>
+      <c r="L29" s="105"/>
+      <c r="M29" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="N29" s="112"/>
-      <c r="O29" s="112"/>
-      <c r="P29" s="112"/>
-      <c r="Q29" s="112"/>
-      <c r="R29" s="112"/>
-      <c r="S29" s="112"/>
-      <c r="T29" s="112"/>
-      <c r="U29" s="112"/>
-      <c r="V29" s="112"/>
-      <c r="W29" s="112"/>
-      <c r="X29" s="113"/>
-      <c r="Y29" s="114" t="s">
+      <c r="N29" s="110"/>
+      <c r="O29" s="110"/>
+      <c r="P29" s="110"/>
+      <c r="Q29" s="110"/>
+      <c r="R29" s="110"/>
+      <c r="S29" s="110"/>
+      <c r="T29" s="110"/>
+      <c r="U29" s="110"/>
+      <c r="V29" s="110"/>
+      <c r="W29" s="110"/>
+      <c r="X29" s="111"/>
+      <c r="Y29" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="Z29" s="114"/>
-      <c r="AA29" s="114"/>
-      <c r="AB29" s="114"/>
-      <c r="AC29" s="114"/>
-      <c r="AD29" s="114"/>
-      <c r="AE29" s="114"/>
+      <c r="Z29" s="112"/>
+      <c r="AA29" s="112"/>
+      <c r="AB29" s="112"/>
+      <c r="AC29" s="112"/>
+      <c r="AD29" s="112"/>
+      <c r="AE29" s="112"/>
     </row>
     <row r="30" spans="1:31" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
@@ -18333,6 +18333,18 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A11:L11"/>
+    <mergeCell ref="M11:V11"/>
+    <mergeCell ref="A29:L29"/>
+    <mergeCell ref="M29:X29"/>
+    <mergeCell ref="Y29:AE29"/>
+    <mergeCell ref="W11:AC11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="A4:B4"/>
@@ -18341,18 +18353,6 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="M11:V11"/>
-    <mergeCell ref="A29:L29"/>
-    <mergeCell ref="M29:X29"/>
-    <mergeCell ref="Y29:AE29"/>
-    <mergeCell ref="W11:AC11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18384,20 +18384,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="101"/>
+      <c r="B1" s="114"/>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="100" t="s">
+      <c r="F1" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="101"/>
+      <c r="G1" s="114"/>
       <c r="H1" s="8" t="s">
         <v>1</v>
       </c>
@@ -18494,10 +18494,10 @@
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="105"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="6">
         <v>12</v>
       </c>
@@ -18516,10 +18516,10 @@
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="105"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="7">
         <v>0.53984146967987301</v>
       </c>
@@ -18582,41 +18582,41 @@
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="106" t="s">
+      <c r="A11" s="104" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="106"/>
-      <c r="C11" s="106"/>
-      <c r="D11" s="106"/>
-      <c r="E11" s="106"/>
-      <c r="F11" s="106"/>
-      <c r="G11" s="106"/>
-      <c r="H11" s="106"/>
-      <c r="I11" s="106"/>
-      <c r="J11" s="106"/>
-      <c r="K11" s="106"/>
-      <c r="L11" s="106"/>
-      <c r="M11" s="108" t="s">
+      <c r="B11" s="104"/>
+      <c r="C11" s="104"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="104"/>
+      <c r="F11" s="104"/>
+      <c r="G11" s="104"/>
+      <c r="H11" s="104"/>
+      <c r="I11" s="104"/>
+      <c r="J11" s="104"/>
+      <c r="K11" s="104"/>
+      <c r="L11" s="104"/>
+      <c r="M11" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="N11" s="109"/>
-      <c r="O11" s="109"/>
-      <c r="P11" s="109"/>
-      <c r="Q11" s="109"/>
-      <c r="R11" s="109"/>
-      <c r="S11" s="109"/>
-      <c r="T11" s="109"/>
-      <c r="U11" s="109"/>
-      <c r="V11" s="110"/>
-      <c r="W11" s="114" t="s">
+      <c r="N11" s="107"/>
+      <c r="O11" s="107"/>
+      <c r="P11" s="107"/>
+      <c r="Q11" s="107"/>
+      <c r="R11" s="107"/>
+      <c r="S11" s="107"/>
+      <c r="T11" s="107"/>
+      <c r="U11" s="107"/>
+      <c r="V11" s="108"/>
+      <c r="W11" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="X11" s="114"/>
-      <c r="Y11" s="114"/>
-      <c r="Z11" s="114"/>
-      <c r="AA11" s="114"/>
-      <c r="AB11" s="114"/>
-      <c r="AC11" s="114"/>
+      <c r="X11" s="112"/>
+      <c r="Y11" s="112"/>
+      <c r="Z11" s="112"/>
+      <c r="AA11" s="112"/>
+      <c r="AB11" s="112"/>
+      <c r="AC11" s="112"/>
     </row>
     <row r="12" spans="1:29" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
@@ -19547,43 +19547,43 @@
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A29" s="107" t="s">
+      <c r="A29" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="107"/>
-      <c r="C29" s="107"/>
-      <c r="D29" s="107"/>
-      <c r="E29" s="107"/>
-      <c r="F29" s="107"/>
-      <c r="G29" s="107"/>
-      <c r="H29" s="107"/>
-      <c r="I29" s="107"/>
-      <c r="J29" s="107"/>
-      <c r="K29" s="107"/>
-      <c r="L29" s="107"/>
-      <c r="M29" s="111" t="s">
+      <c r="B29" s="105"/>
+      <c r="C29" s="105"/>
+      <c r="D29" s="105"/>
+      <c r="E29" s="105"/>
+      <c r="F29" s="105"/>
+      <c r="G29" s="105"/>
+      <c r="H29" s="105"/>
+      <c r="I29" s="105"/>
+      <c r="J29" s="105"/>
+      <c r="K29" s="105"/>
+      <c r="L29" s="105"/>
+      <c r="M29" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="N29" s="112"/>
-      <c r="O29" s="112"/>
-      <c r="P29" s="112"/>
-      <c r="Q29" s="112"/>
-      <c r="R29" s="112"/>
-      <c r="S29" s="112"/>
-      <c r="T29" s="112"/>
-      <c r="U29" s="112"/>
-      <c r="V29" s="112"/>
-      <c r="W29" s="112"/>
-      <c r="X29" s="113"/>
-      <c r="Y29" s="114" t="s">
+      <c r="N29" s="110"/>
+      <c r="O29" s="110"/>
+      <c r="P29" s="110"/>
+      <c r="Q29" s="110"/>
+      <c r="R29" s="110"/>
+      <c r="S29" s="110"/>
+      <c r="T29" s="110"/>
+      <c r="U29" s="110"/>
+      <c r="V29" s="110"/>
+      <c r="W29" s="110"/>
+      <c r="X29" s="111"/>
+      <c r="Y29" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="Z29" s="114"/>
-      <c r="AA29" s="114"/>
-      <c r="AB29" s="114"/>
-      <c r="AC29" s="114"/>
-      <c r="AD29" s="114"/>
-      <c r="AE29" s="114"/>
+      <c r="Z29" s="112"/>
+      <c r="AA29" s="112"/>
+      <c r="AB29" s="112"/>
+      <c r="AC29" s="112"/>
+      <c r="AD29" s="112"/>
+      <c r="AE29" s="112"/>
     </row>
     <row r="30" spans="1:31" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
@@ -20604,6 +20604,18 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="M29:X29"/>
     <mergeCell ref="A29:L29"/>
     <mergeCell ref="M11:V11"/>
@@ -20612,18 +20624,6 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="W11:AC11"/>
     <mergeCell ref="Y29:AE29"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -20654,20 +20654,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="101"/>
+      <c r="B1" s="114"/>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="100" t="s">
+      <c r="F1" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="101"/>
+      <c r="G1" s="114"/>
       <c r="H1" s="8" t="s">
         <v>1</v>
       </c>
@@ -20764,10 +20764,10 @@
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="105"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="6">
         <v>12</v>
       </c>
@@ -20786,10 +20786,10 @@
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="105"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="7">
         <v>0.36291863507890598</v>
       </c>
@@ -20866,27 +20866,27 @@
       <c r="J11" s="116"/>
       <c r="K11" s="116"/>
       <c r="L11" s="117"/>
-      <c r="M11" s="108" t="s">
+      <c r="M11" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="N11" s="109"/>
-      <c r="O11" s="109"/>
-      <c r="P11" s="109"/>
-      <c r="Q11" s="109"/>
-      <c r="R11" s="109"/>
-      <c r="S11" s="109"/>
-      <c r="T11" s="109"/>
-      <c r="U11" s="109"/>
-      <c r="V11" s="110"/>
-      <c r="W11" s="114" t="s">
+      <c r="N11" s="107"/>
+      <c r="O11" s="107"/>
+      <c r="P11" s="107"/>
+      <c r="Q11" s="107"/>
+      <c r="R11" s="107"/>
+      <c r="S11" s="107"/>
+      <c r="T11" s="107"/>
+      <c r="U11" s="107"/>
+      <c r="V11" s="108"/>
+      <c r="W11" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="X11" s="114"/>
-      <c r="Y11" s="114"/>
-      <c r="Z11" s="114"/>
-      <c r="AA11" s="114"/>
-      <c r="AB11" s="114"/>
-      <c r="AC11" s="114"/>
+      <c r="X11" s="112"/>
+      <c r="Y11" s="112"/>
+      <c r="Z11" s="112"/>
+      <c r="AA11" s="112"/>
+      <c r="AB11" s="112"/>
+      <c r="AC11" s="112"/>
     </row>
     <row r="12" spans="1:29" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
@@ -21665,29 +21665,29 @@
       <c r="J26" s="118"/>
       <c r="K26" s="118"/>
       <c r="L26" s="119"/>
-      <c r="M26" s="111" t="s">
+      <c r="M26" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="N26" s="112"/>
-      <c r="O26" s="112"/>
-      <c r="P26" s="112"/>
-      <c r="Q26" s="112"/>
-      <c r="R26" s="112"/>
-      <c r="S26" s="112"/>
-      <c r="T26" s="112"/>
-      <c r="U26" s="112"/>
-      <c r="V26" s="112"/>
-      <c r="W26" s="112"/>
-      <c r="X26" s="113"/>
-      <c r="Y26" s="114" t="s">
+      <c r="N26" s="110"/>
+      <c r="O26" s="110"/>
+      <c r="P26" s="110"/>
+      <c r="Q26" s="110"/>
+      <c r="R26" s="110"/>
+      <c r="S26" s="110"/>
+      <c r="T26" s="110"/>
+      <c r="U26" s="110"/>
+      <c r="V26" s="110"/>
+      <c r="W26" s="110"/>
+      <c r="X26" s="111"/>
+      <c r="Y26" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="Z26" s="114"/>
-      <c r="AA26" s="114"/>
-      <c r="AB26" s="114"/>
-      <c r="AC26" s="114"/>
-      <c r="AD26" s="114"/>
-      <c r="AE26" s="114"/>
+      <c r="Z26" s="112"/>
+      <c r="AA26" s="112"/>
+      <c r="AB26" s="112"/>
+      <c r="AC26" s="112"/>
+      <c r="AD26" s="112"/>
+      <c r="AE26" s="112"/>
     </row>
     <row r="27" spans="1:31" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
@@ -22710,18 +22710,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="F6:G6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="A11:L11"/>
@@ -22730,6 +22718,18 @@
     <mergeCell ref="M26:X26"/>
     <mergeCell ref="W11:AC11"/>
     <mergeCell ref="Y26:AE26"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -22760,20 +22760,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="101"/>
+      <c r="B1" s="114"/>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="100" t="s">
+      <c r="F1" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="101"/>
+      <c r="G1" s="114"/>
       <c r="H1" s="8" t="s">
         <v>1</v>
       </c>
@@ -22870,10 +22870,10 @@
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="105"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="6">
         <v>12</v>
       </c>
@@ -22892,10 +22892,10 @@
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="105"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="7">
         <v>0.36291863507890598</v>
       </c>
@@ -22971,27 +22971,27 @@
       <c r="J11" s="116"/>
       <c r="K11" s="116"/>
       <c r="L11" s="117"/>
-      <c r="M11" s="108" t="s">
+      <c r="M11" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="N11" s="109"/>
-      <c r="O11" s="109"/>
-      <c r="P11" s="109"/>
-      <c r="Q11" s="109"/>
-      <c r="R11" s="109"/>
-      <c r="S11" s="109"/>
-      <c r="T11" s="109"/>
-      <c r="U11" s="109"/>
-      <c r="V11" s="110"/>
-      <c r="W11" s="114" t="s">
+      <c r="N11" s="107"/>
+      <c r="O11" s="107"/>
+      <c r="P11" s="107"/>
+      <c r="Q11" s="107"/>
+      <c r="R11" s="107"/>
+      <c r="S11" s="107"/>
+      <c r="T11" s="107"/>
+      <c r="U11" s="107"/>
+      <c r="V11" s="108"/>
+      <c r="W11" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="X11" s="114"/>
-      <c r="Y11" s="114"/>
-      <c r="Z11" s="114"/>
-      <c r="AA11" s="114"/>
-      <c r="AB11" s="114"/>
-      <c r="AC11" s="114"/>
+      <c r="X11" s="112"/>
+      <c r="Y11" s="112"/>
+      <c r="Z11" s="112"/>
+      <c r="AA11" s="112"/>
+      <c r="AB11" s="112"/>
+      <c r="AC11" s="112"/>
     </row>
     <row r="12" spans="1:29" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
@@ -24100,29 +24100,29 @@
       <c r="J31" s="118"/>
       <c r="K31" s="118"/>
       <c r="L31" s="119"/>
-      <c r="M31" s="111" t="s">
+      <c r="M31" s="109" t="s">
         <v>66</v>
       </c>
-      <c r="N31" s="112"/>
-      <c r="O31" s="112"/>
-      <c r="P31" s="112"/>
-      <c r="Q31" s="112"/>
-      <c r="R31" s="112"/>
-      <c r="S31" s="112"/>
-      <c r="T31" s="112"/>
-      <c r="U31" s="112"/>
-      <c r="V31" s="112"/>
-      <c r="W31" s="112"/>
-      <c r="X31" s="113"/>
-      <c r="Y31" s="114" t="s">
+      <c r="N31" s="110"/>
+      <c r="O31" s="110"/>
+      <c r="P31" s="110"/>
+      <c r="Q31" s="110"/>
+      <c r="R31" s="110"/>
+      <c r="S31" s="110"/>
+      <c r="T31" s="110"/>
+      <c r="U31" s="110"/>
+      <c r="V31" s="110"/>
+      <c r="W31" s="110"/>
+      <c r="X31" s="111"/>
+      <c r="Y31" s="112" t="s">
         <v>88</v>
       </c>
-      <c r="Z31" s="114"/>
-      <c r="AA31" s="114"/>
-      <c r="AB31" s="114"/>
-      <c r="AC31" s="114"/>
-      <c r="AD31" s="114"/>
-      <c r="AE31" s="114"/>
+      <c r="Z31" s="112"/>
+      <c r="AA31" s="112"/>
+      <c r="AB31" s="112"/>
+      <c r="AC31" s="112"/>
+      <c r="AD31" s="112"/>
+      <c r="AE31" s="112"/>
     </row>
     <row r="32" spans="1:31" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
@@ -25145,6 +25145,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="F3:G3"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="A6:B6"/>
@@ -25157,14 +25165,6 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="W11:AC11"/>
     <mergeCell ref="Y31:AE31"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -25519,20 +25519,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="101"/>
+      <c r="B1" s="114"/>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="100" t="s">
+      <c r="F1" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="101"/>
+      <c r="G1" s="114"/>
       <c r="H1" s="8" t="s">
         <v>1</v>
       </c>
@@ -25629,10 +25629,10 @@
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="105"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="6">
         <v>12</v>
       </c>
@@ -25651,10 +25651,10 @@
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="105"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="7">
         <v>0.235897112801289</v>
       </c>
@@ -25730,18 +25730,18 @@
       <c r="J11" s="123"/>
       <c r="K11" s="123"/>
       <c r="L11" s="124"/>
-      <c r="M11" s="108" t="s">
+      <c r="M11" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="N11" s="109"/>
-      <c r="O11" s="109"/>
-      <c r="P11" s="109"/>
-      <c r="Q11" s="109"/>
-      <c r="R11" s="109"/>
-      <c r="S11" s="109"/>
-      <c r="T11" s="109"/>
-      <c r="U11" s="109"/>
-      <c r="V11" s="110"/>
+      <c r="N11" s="107"/>
+      <c r="O11" s="107"/>
+      <c r="P11" s="107"/>
+      <c r="Q11" s="107"/>
+      <c r="R11" s="107"/>
+      <c r="S11" s="107"/>
+      <c r="T11" s="107"/>
+      <c r="U11" s="107"/>
+      <c r="V11" s="108"/>
     </row>
     <row r="12" spans="1:22" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
@@ -27340,24 +27340,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="M11:V11"/>
+    <mergeCell ref="M29:X29"/>
+    <mergeCell ref="A11:L11"/>
+    <mergeCell ref="A29:L29"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="M11:V11"/>
-    <mergeCell ref="M29:X29"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="A29:L29"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="F7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -27386,20 +27386,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="101"/>
+      <c r="B1" s="114"/>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="100" t="s">
+      <c r="F1" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="101"/>
+      <c r="G1" s="114"/>
       <c r="H1" s="8" t="s">
         <v>1</v>
       </c>
@@ -27496,10 +27496,10 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="100" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="105"/>
+      <c r="B6" s="101"/>
       <c r="C6" s="6">
         <v>12</v>
       </c>
@@ -27518,10 +27518,10 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="105"/>
+      <c r="B7" s="101"/>
       <c r="C7" s="6">
         <v>0.54</v>
       </c>

</xml_diff>